<commit_message>
Added main flask app. Added comments.
</commit_message>
<xml_diff>
--- a/Docs/waffles.xlsx
+++ b/Docs/waffles.xlsx
@@ -569,7 +569,7 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Как испечь вафли хрустящие в вафельнице? Подготовьте необходимые продукты. Из данного количества у меня получилось 8 штук диаметром около 10 см.</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Масло положите в сотейник с толстым дном. Растопите его на маленьком огне на плите, на водяной бане либо в микроволновке.</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Добавьте в теплое масло сахар. Перемешайте венчиком до полного растворения сахара. От тепла сахар довольно быстро растает.</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Добавьте в масло яйцо. Предварительно все-таки проверьте масло, не горячее ли оно, иначе яйцо может свариться. Перемешайте яйцо с маслом до однородности.</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Всыпьте муку, добавьте ванилин.</t>
         </is>
       </c>
     </row>
@@ -619,7 +619,7 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Перемешайте массу венчиком до состояния гладкого однородного теста.</t>
         </is>
       </c>
     </row>
@@ -629,7 +629,7 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Разогрейте вафельницу по инструкции к ней. У меня очень старая, еще советских времен электровафельница. Она может и не очень красивая, но печет замечательно! Я не смазываю вафельницу маслом, в тесте достаточно жира, да и к ней уже давно ничего не прилипает. Но вы смотрите по своей модели. Выкладывайте тесто по столовой ложке. Можно класть немного меньше теста, тогда вафли будут меньше и их получится больше.</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>[Ошибка форматирования шага: 'response_xlsx' object has no attribute '_format_step_description']</t>
+          <t>Пеките вафли несколько минут до золотистого цвета. Осторожно откройте вафельницу, она очень горячая! Снимите вафлю лопаткой. Горячая она очень мягкая, как блинчик.</t>
         </is>
       </c>
     </row>

</xml_diff>